<commit_message>
updated SYDATA-Work order testcases
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/RMA Complete Flow(Issue Credit)-SO TO RMA Receipt To Create Credit Memo.xlsx
+++ b/templates/AutomationOrg/RMA Complete Flow(Issue Credit)-SO TO RMA Receipt To Create Credit Memo.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="282">
   <si>
     <t>API Mode</t>
   </si>
@@ -807,6 +807,87 @@
   </si>
   <si>
     <t>RMA-J098-1-3</t>
+  </si>
+  <si>
+    <t>RMA-8XKB-001</t>
+  </si>
+  <si>
+    <t>RMA-8XKB-002</t>
+  </si>
+  <si>
+    <t>RMA-8XKB-003</t>
+  </si>
+  <si>
+    <t>a7s5f000000xL0iAAE</t>
+  </si>
+  <si>
+    <t>RMA-8XKB-1-1</t>
+  </si>
+  <si>
+    <t>a7s5f000000xL0jAAE</t>
+  </si>
+  <si>
+    <t>RMA-8XKB-1-2</t>
+  </si>
+  <si>
+    <t>a7s5f000000xL0kAAE</t>
+  </si>
+  <si>
+    <t>RMA-8XKB-1-3</t>
+  </si>
+  <si>
+    <t>RMA-3STF-001</t>
+  </si>
+  <si>
+    <t>RMA-3STF-002</t>
+  </si>
+  <si>
+    <t>RMA-3STF-003</t>
+  </si>
+  <si>
+    <t>a7s5f000000xL2PAAU</t>
+  </si>
+  <si>
+    <t>RMA-3STF-1-1</t>
+  </si>
+  <si>
+    <t>a7s5f000000xL2QAAU</t>
+  </si>
+  <si>
+    <t>RMA-3STF-1-2</t>
+  </si>
+  <si>
+    <t>a7s5f000000xL2RAAU</t>
+  </si>
+  <si>
+    <t>RMA-3STF-1-3</t>
+  </si>
+  <si>
+    <t>RMA-MG41-001</t>
+  </si>
+  <si>
+    <t>RMA-MG41-002</t>
+  </si>
+  <si>
+    <t>RMA-MG41-003</t>
+  </si>
+  <si>
+    <t>a7s5f000000xL33AAE</t>
+  </si>
+  <si>
+    <t>RMA-MG41-1-1</t>
+  </si>
+  <si>
+    <t>a7s5f000000xL34AAE</t>
+  </si>
+  <si>
+    <t>RMA-MG41-1-2</t>
+  </si>
+  <si>
+    <t>a7s5f000000xL35AAE</t>
+  </si>
+  <si>
+    <t>RMA-MG41-1-3</t>
   </si>
 </sst>
 </file>
@@ -816,7 +897,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="255" x14ac:knownFonts="1">
+  <fonts count="291" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -836,6 +917,222 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -2358,7 +2655,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="127">
+  <borders count="145">
     <border>
       <left/>
       <right/>
@@ -2744,11 +3041,65 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="255">
+  <cellXfs count="291">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
@@ -3002,8 +3353,44 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="124" fillId="0" fontId="250" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="251" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="125" fillId="0" fontId="252" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="253" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="254" fillId="0" borderId="126" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="253" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="126" fillId="0" fontId="254" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="255" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="127" fillId="0" fontId="256" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="257" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="128" fillId="0" fontId="258" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="259" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="129" fillId="0" fontId="260" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="261" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="130" fillId="0" fontId="262" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="263" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="131" fillId="0" fontId="264" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="265" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="132" fillId="0" fontId="266" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="267" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="133" fillId="0" fontId="268" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="269" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="134" fillId="0" fontId="270" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="271" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="135" fillId="0" fontId="272" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="273" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="136" fillId="0" fontId="274" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="275" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="137" fillId="0" fontId="276" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="277" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="138" fillId="0" fontId="278" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="279" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="139" fillId="0" fontId="280" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="281" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="140" fillId="0" fontId="282" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="283" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="141" fillId="0" fontId="284" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="285" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="142" fillId="0" fontId="286" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="287" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="143" fillId="0" fontId="288" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="289" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="290" fillId="0" borderId="144" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -3790,12 +4177,12 @@
     <col min="2" max="2" bestFit="true" customWidth="true" width="39.7578125" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="19.2265625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="20.5078125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="15.4765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.6796875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.57421875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.1328125" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="11.4921875" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="14.515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="21.19921875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.26953125" collapsed="true"/>
     <col min="11" max="12" bestFit="true" customWidth="true" width="21.21875" collapsed="true"/>
   </cols>
   <sheetData>
@@ -3845,10 +4232,10 @@
         <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>246</v>
+        <v>273</v>
       </c>
       <c r="F2" t="s">
-        <v>250</v>
+        <v>277</v>
       </c>
       <c r="G2" t="s">
         <v>68</v>
@@ -3857,7 +4244,7 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>249</v>
+        <v>276</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -3874,10 +4261,10 @@
         <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>247</v>
+        <v>274</v>
       </c>
       <c r="F3" t="s">
-        <v>252</v>
+        <v>279</v>
       </c>
       <c r="G3" t="s">
         <v>68</v>
@@ -3886,7 +4273,7 @@
         <v>37</v>
       </c>
       <c r="J3" t="s">
-        <v>251</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -3903,10 +4290,10 @@
         <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>248</v>
+        <v>275</v>
       </c>
       <c r="F4" t="s">
-        <v>254</v>
+        <v>281</v>
       </c>
       <c r="G4" t="s">
         <v>68</v>
@@ -3915,7 +4302,7 @@
         <v>37</v>
       </c>
       <c r="J4" t="s">
-        <v>253</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimized WO test cases|Changes related to Excel Files
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/RMA Complete Flow(Issue Credit)-SO TO RMA Receipt To Create Credit Memo.xlsx
+++ b/templates/AutomationOrg/RMA Complete Flow(Issue Credit)-SO TO RMA Receipt To Create Credit Memo.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="318">
   <si>
     <t>API Mode</t>
   </si>
@@ -969,6 +969,33 @@
   </si>
   <si>
     <t>RMA-BR6P-1-3</t>
+  </si>
+  <si>
+    <t>RMA-CFAT-001</t>
+  </si>
+  <si>
+    <t>RMA-CFAT-002</t>
+  </si>
+  <si>
+    <t>RMA-CFAT-003</t>
+  </si>
+  <si>
+    <t>a7s5f000000xLLHAA2</t>
+  </si>
+  <si>
+    <t>RMA-CFAT-1-1</t>
+  </si>
+  <si>
+    <t>a7s5f000000xLLIAA2</t>
+  </si>
+  <si>
+    <t>RMA-CFAT-1-2</t>
+  </si>
+  <si>
+    <t>a7s5f000000xLLJAA2</t>
+  </si>
+  <si>
+    <t>RMA-CFAT-1-3</t>
   </si>
 </sst>
 </file>
@@ -978,7 +1005,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="327" x14ac:knownFonts="1">
+  <fonts count="339" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -998,6 +1025,78 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -2952,7 +3051,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="163">
+  <borders count="169">
     <border>
       <left/>
       <right/>
@@ -3446,11 +3545,29 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="327">
+  <cellXfs count="339">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
@@ -3776,8 +3893,20 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="160" fillId="0" fontId="322" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="323" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="161" fillId="0" fontId="324" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="325" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="326" fillId="0" borderId="162" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="325" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="162" fillId="0" fontId="326" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="327" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="163" fillId="0" fontId="328" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="329" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="164" fillId="0" fontId="330" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="331" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="165" fillId="0" fontId="332" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="333" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="166" fillId="0" fontId="334" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="335" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="167" fillId="0" fontId="336" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="337" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="338" fillId="0" borderId="168" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -4565,11 +4694,11 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="19.2265625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="20.5078125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.4765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.27734375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.1640625" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="11.4921875" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="14.515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="21.03515625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="20.375" collapsed="true"/>
     <col min="11" max="12" bestFit="true" customWidth="true" width="21.21875" collapsed="true"/>
   </cols>
   <sheetData>
@@ -4619,10 +4748,10 @@
         <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="F2" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="G2" t="s">
         <v>68</v>
@@ -4631,7 +4760,7 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -4648,10 +4777,10 @@
         <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="F3" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="G3" t="s">
         <v>68</v>
@@ -4660,7 +4789,7 @@
         <v>37</v>
       </c>
       <c r="J3" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -4677,10 +4806,10 @@
         <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="F4" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="G4" t="s">
         <v>68</v>
@@ -4689,7 +4818,7 @@
         <v>37</v>
       </c>
       <c r="J4" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Work Order templates and other fixes.
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/RMA Complete Flow(Issue Credit)-SO TO RMA Receipt To Create Credit Memo.xlsx
+++ b/templates/AutomationOrg/RMA Complete Flow(Issue Credit)-SO TO RMA Receipt To Create Credit Memo.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="527">
   <si>
     <t>API Mode</t>
   </si>
@@ -1515,6 +1515,114 @@
   </si>
   <si>
     <t>RMA-391D-1-3</t>
+  </si>
+  <si>
+    <t>RMA-478W-001</t>
+  </si>
+  <si>
+    <t>RMA-478W-002</t>
+  </si>
+  <si>
+    <t>RMA-478W-003</t>
+  </si>
+  <si>
+    <t>a7s5f000000xMAPAA2</t>
+  </si>
+  <si>
+    <t>RMA-478W-1-1</t>
+  </si>
+  <si>
+    <t>a7s5f000000xMAQAA2</t>
+  </si>
+  <si>
+    <t>RMA-478W-1-2</t>
+  </si>
+  <si>
+    <t>a7s5f000000xMARAA2</t>
+  </si>
+  <si>
+    <t>RMA-478W-1-3</t>
+  </si>
+  <si>
+    <t>RMA-K3US-001</t>
+  </si>
+  <si>
+    <t>RMA-K3US-002</t>
+  </si>
+  <si>
+    <t>RMA-K3US-003</t>
+  </si>
+  <si>
+    <t>a7s5f000000xMrTAAU</t>
+  </si>
+  <si>
+    <t>RMA-K3US-1-1</t>
+  </si>
+  <si>
+    <t>a7s5f000000xMrUAAU</t>
+  </si>
+  <si>
+    <t>RMA-K3US-1-2</t>
+  </si>
+  <si>
+    <t>a7s5f000000xMrVAAU</t>
+  </si>
+  <si>
+    <t>RMA-K3US-1-3</t>
+  </si>
+  <si>
+    <t>RMA-VCUF-001</t>
+  </si>
+  <si>
+    <t>RMA-VCUF-002</t>
+  </si>
+  <si>
+    <t>RMA-VCUF-003</t>
+  </si>
+  <si>
+    <t>a7s5f000000xMrdAAE</t>
+  </si>
+  <si>
+    <t>RMA-VCUF-1-1</t>
+  </si>
+  <si>
+    <t>a7s5f000000xMreAAE</t>
+  </si>
+  <si>
+    <t>RMA-VCUF-1-2</t>
+  </si>
+  <si>
+    <t>a7s5f000000xMrfAAE</t>
+  </si>
+  <si>
+    <t>RMA-VCUF-1-3</t>
+  </si>
+  <si>
+    <t>RMA-PU7Q-001</t>
+  </si>
+  <si>
+    <t>RMA-PU7Q-002</t>
+  </si>
+  <si>
+    <t>RMA-PU7Q-003</t>
+  </si>
+  <si>
+    <t>a7s5f000000xMsgAAE</t>
+  </si>
+  <si>
+    <t>RMA-PU7Q-1-1</t>
+  </si>
+  <si>
+    <t>a7s5f000000xMshAAE</t>
+  </si>
+  <si>
+    <t>RMA-PU7Q-1-2</t>
+  </si>
+  <si>
+    <t>a7s5f000000xMsiAAE</t>
+  </si>
+  <si>
+    <t>RMA-PU7Q-1-3</t>
   </si>
 </sst>
 </file>
@@ -1524,7 +1632,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="575" x14ac:knownFonts="1">
+  <fonts count="623" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1544,6 +1652,294 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -4986,7 +5382,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="287">
+  <borders count="311">
     <border>
       <left/>
       <right/>
@@ -5852,11 +6248,83 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="575">
+  <cellXfs count="623">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
@@ -6430,8 +6898,56 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="284" fillId="0" fontId="570" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="571" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="285" fillId="0" fontId="572" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="573" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="574" fillId="0" borderId="286" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="573" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="286" fillId="0" fontId="574" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="575" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="287" fillId="0" fontId="576" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="577" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="288" fillId="0" fontId="578" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="579" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="289" fillId="0" fontId="580" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="581" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="290" fillId="0" fontId="582" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="583" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="291" fillId="0" fontId="584" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="585" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="292" fillId="0" fontId="586" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="587" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="293" fillId="0" fontId="588" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="589" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="294" fillId="0" fontId="590" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="591" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="295" fillId="0" fontId="592" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="593" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="296" fillId="0" fontId="594" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="595" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="297" fillId="0" fontId="596" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="597" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="298" fillId="0" fontId="598" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="599" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="299" fillId="0" fontId="600" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="601" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="300" fillId="0" fontId="602" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="603" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="301" fillId="0" fontId="604" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="605" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="302" fillId="0" fontId="606" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="607" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="303" fillId="0" fontId="608" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="609" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="304" fillId="0" fontId="610" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="611" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="305" fillId="0" fontId="612" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="613" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="306" fillId="0" fontId="614" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="615" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="307" fillId="0" fontId="616" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="617" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="308" fillId="0" fontId="618" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="619" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="309" fillId="0" fontId="620" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="621" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="622" fillId="0" borderId="310" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -7219,11 +7735,11 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="19.2265625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="20.5078125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.4765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.77734375" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="11.4921875" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="14.515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="20.44921875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="21.01171875" collapsed="true"/>
     <col min="11" max="12" bestFit="true" customWidth="true" width="21.21875" collapsed="true"/>
   </cols>
   <sheetData>
@@ -7273,10 +7789,10 @@
         <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>482</v>
+        <v>518</v>
       </c>
       <c r="F2" t="s">
-        <v>486</v>
+        <v>522</v>
       </c>
       <c r="G2" t="s">
         <v>68</v>
@@ -7285,7 +7801,7 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>485</v>
+        <v>521</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -7302,10 +7818,10 @@
         <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>483</v>
+        <v>519</v>
       </c>
       <c r="F3" t="s">
-        <v>488</v>
+        <v>524</v>
       </c>
       <c r="G3" t="s">
         <v>68</v>
@@ -7314,7 +7830,7 @@
         <v>37</v>
       </c>
       <c r="J3" t="s">
-        <v>487</v>
+        <v>523</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -7331,10 +7847,10 @@
         <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>484</v>
+        <v>520</v>
       </c>
       <c r="F4" t="s">
-        <v>490</v>
+        <v>526</v>
       </c>
       <c r="G4" t="s">
         <v>68</v>
@@ -7343,7 +7859,7 @@
         <v>37</v>
       </c>
       <c r="J4" t="s">
-        <v>489</v>
+        <v>525</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Test plan/Added Custom API-Switch TO Lightning OR classic/Template Changes/WIP-LUI_Work Order
</commit_message>
<xml_diff>
--- a/templates/AutomationOrg/RMA Complete Flow(Issue Credit)-SO TO RMA Receipt To Create Credit Memo.xlsx
+++ b/templates/AutomationOrg/RMA Complete Flow(Issue Credit)-SO TO RMA Receipt To Create Credit Memo.xlsx
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="536">
   <si>
     <t>API Mode</t>
   </si>
@@ -1623,6 +1623,33 @@
   </si>
   <si>
     <t>RMA-PU7Q-1-3</t>
+  </si>
+  <si>
+    <t>RMA-Q190-001</t>
+  </si>
+  <si>
+    <t>RMA-Q190-002</t>
+  </si>
+  <si>
+    <t>RMA-Q190-003</t>
+  </si>
+  <si>
+    <t>a7s5f000000xNY8AAM</t>
+  </si>
+  <si>
+    <t>RMA-Q190-1-1</t>
+  </si>
+  <si>
+    <t>a7s5f000000xNY9AAM</t>
+  </si>
+  <si>
+    <t>RMA-Q190-1-2</t>
+  </si>
+  <si>
+    <t>a7s5f000000xNYAAA2</t>
+  </si>
+  <si>
+    <t>RMA-Q190-1-3</t>
   </si>
 </sst>
 </file>
@@ -1632,7 +1659,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="623" x14ac:knownFonts="1">
+  <fonts count="635" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1652,6 +1679,78 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="12.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="10.0"/>
+      <color indexed="10"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -5382,7 +5481,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="311">
+  <borders count="317">
     <border>
       <left/>
       <right/>
@@ -6320,11 +6419,29 @@
     <border>
       <bottom style="thin"/>
     </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="623">
+  <cellXfs count="635">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
     <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
@@ -6946,8 +7063,20 @@
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="308" fillId="0" fontId="618" numFmtId="49" xfId="0"/>
     <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="619" numFmtId="164" xfId="0"/>
     <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="309" fillId="0" fontId="620" numFmtId="49" xfId="0"/>
-    <xf numFmtId="164" fontId="621" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
-    <xf numFmtId="49" fontId="622" fillId="0" borderId="310" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="621" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="310" fillId="0" fontId="622" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="623" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="311" fillId="0" fontId="624" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="625" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="312" fillId="0" fontId="626" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="627" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="313" fillId="0" fontId="628" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="629" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="314" fillId="0" fontId="630" numFmtId="49" xfId="0"/>
+    <xf applyFont="true" applyNumberFormat="true" borderId="0" fillId="0" fontId="631" numFmtId="164" xfId="0"/>
+    <xf applyBorder="true" applyFont="true" applyNumberFormat="true" borderId="315" fillId="0" fontId="632" numFmtId="49" xfId="0"/>
+    <xf numFmtId="164" fontId="633" fillId="0" borderId="0" xfId="0" applyFont="true" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="634" fillId="0" borderId="316" xfId="0" applyBorder="true" applyNumberFormat="true" applyFont="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -7735,11 +7864,11 @@
     <col min="3" max="3" bestFit="true" customWidth="true" width="19.2265625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="20.5078125" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.4765625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.77734375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.4609375" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="11.4921875" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="14.515625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="21.01171875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="21.52734375" collapsed="true"/>
     <col min="11" max="12" bestFit="true" customWidth="true" width="21.21875" collapsed="true"/>
   </cols>
   <sheetData>
@@ -7789,10 +7918,10 @@
         <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>518</v>
+        <v>527</v>
       </c>
       <c r="F2" t="s">
-        <v>522</v>
+        <v>531</v>
       </c>
       <c r="G2" t="s">
         <v>68</v>
@@ -7801,7 +7930,7 @@
         <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>521</v>
+        <v>530</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -7818,10 +7947,10 @@
         <v>26</v>
       </c>
       <c r="E3" t="s">
-        <v>519</v>
+        <v>528</v>
       </c>
       <c r="F3" t="s">
-        <v>524</v>
+        <v>533</v>
       </c>
       <c r="G3" t="s">
         <v>68</v>
@@ -7830,7 +7959,7 @@
         <v>37</v>
       </c>
       <c r="J3" t="s">
-        <v>523</v>
+        <v>532</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -7847,10 +7976,10 @@
         <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>520</v>
+        <v>529</v>
       </c>
       <c r="F4" t="s">
-        <v>526</v>
+        <v>535</v>
       </c>
       <c r="G4" t="s">
         <v>68</v>
@@ -7859,7 +7988,7 @@
         <v>37</v>
       </c>
       <c r="J4" t="s">
-        <v>525</v>
+        <v>534</v>
       </c>
     </row>
   </sheetData>

</xml_diff>